<commit_message>
Start of keynote presentation
</commit_message>
<xml_diff>
--- a/HML.xlsx
+++ b/HML.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="22160" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="1520" yWindow="460" windowWidth="27200" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,23 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
-  <si>
-    <t>Coord1</t>
-  </si>
-  <si>
-    <t>int x, y</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
   <si>
     <t>Forme</t>
   </si>
   <si>
-    <t>string Couleur</t>
-  </si>
-  <si>
-    <t>unsigned int transparence</t>
-  </si>
-  <si>
     <t>Rectangle</t>
   </si>
   <si>
@@ -50,9 +38,6 @@
     <t>Cercle</t>
   </si>
   <si>
-    <t>unsigned int rayon</t>
-  </si>
-  <si>
     <t>Point</t>
   </si>
   <si>
@@ -62,15 +47,9 @@
     <t>Ligne</t>
   </si>
   <si>
-    <t>Coord2</t>
-  </si>
-  <si>
     <t>Triangle</t>
   </si>
   <si>
-    <t>Coord3</t>
-  </si>
-  <si>
     <t>Cercle_p</t>
   </si>
   <si>
@@ -107,7 +86,91 @@
     <t>vector&lt;unsigned int&gt; m_l</t>
   </si>
   <si>
-    <t>3 lignes</t>
+    <t>Cimage</t>
+  </si>
+  <si>
+    <t>Cligne</t>
+  </si>
+  <si>
+    <t>Cpixel</t>
+  </si>
+  <si>
+    <t>Cbitmap</t>
+  </si>
+  <si>
+    <t>LoadBMP</t>
+  </si>
+  <si>
+    <t>dump</t>
+  </si>
+  <si>
+    <t>CImage *getImage</t>
+  </si>
+  <si>
+    <t>void setImage</t>
+  </si>
+  <si>
+    <t>int size</t>
+  </si>
+  <si>
+    <t>CLigne* getLigne</t>
+  </si>
+  <si>
+    <t>CPixel* getPixel</t>
+  </si>
+  <si>
+    <t>void drawPixel</t>
+  </si>
+  <si>
+    <t>CLigne** liste</t>
+  </si>
+  <si>
+    <t>int taille</t>
+  </si>
+  <si>
+    <t>CPixel** ligne</t>
+  </si>
+  <si>
+    <t>int Red</t>
+  </si>
+  <si>
+    <t>int Green</t>
+  </si>
+  <si>
+    <t>int Blue</t>
+  </si>
+  <si>
+    <t>void RGB</t>
+  </si>
+  <si>
+    <t>CImage *image;</t>
+  </si>
+  <si>
+    <t>&amp; autres</t>
+  </si>
+  <si>
+    <t>string m_couleur</t>
+  </si>
+  <si>
+    <t>Coord m_c1</t>
+  </si>
+  <si>
+    <t>unsigned int m_transparence</t>
+  </si>
+  <si>
+    <t>Coord</t>
+  </si>
+  <si>
+    <t>int m_x, m_y</t>
+  </si>
+  <si>
+    <t>Coord m_c2</t>
+  </si>
+  <si>
+    <t>Coord m_c3</t>
+  </si>
+  <si>
+    <t>unsigned int m_rayon</t>
   </si>
 </sst>
 </file>
@@ -236,13 +299,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>393700</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
@@ -286,13 +349,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>1206500</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>165100</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
@@ -333,14 +396,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>520700</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
+      <xdr:rowOff>115454</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1366212</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
@@ -351,8 +414,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3822700" y="1600200"/>
-          <a:ext cx="2387600" cy="1435100"/>
+          <a:off x="10257367" y="1597121"/>
+          <a:ext cx="3577936" cy="1505912"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -380,16 +443,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
+      <xdr:rowOff>19242</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1385454</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>190501</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -398,8 +461,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2032000" y="1371600"/>
-          <a:ext cx="4178300" cy="1714500"/>
+          <a:off x="6519333" y="1289242"/>
+          <a:ext cx="7335212" cy="1864592"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -427,13 +490,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
@@ -474,13 +537,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>330200</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
@@ -521,13 +584,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>558800</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>558800</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>203200</xdr:rowOff>
@@ -568,13 +631,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -615,13 +678,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
@@ -669,13 +732,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>241300</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
@@ -723,13 +786,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>165100</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>519545</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -768,13 +831,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>519545</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>28863</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>533977</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>86591</xdr:rowOff>
@@ -812,13 +875,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>490682</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>72159</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>938068</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>80241</xdr:rowOff>
@@ -857,13 +920,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>931718</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>210127</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>946150</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>51377</xdr:rowOff>
@@ -901,14 +964,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>923637</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>173182</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1933863</xdr:colOff>
+      <xdr:rowOff>173181</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2347576</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>181264</xdr:rowOff>
     </xdr:to>
@@ -919,8 +982,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="10073410" y="3478068"/>
-          <a:ext cx="1010226" cy="8082"/>
+          <a:off x="14989849" y="3559848"/>
+          <a:ext cx="1423939" cy="8083"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -946,13 +1009,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>418523</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>14431</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>418523</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
@@ -993,13 +1056,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>36945</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>86013</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>392545</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>98713</xdr:rowOff>
@@ -1047,13 +1110,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>477404</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>202045</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>871104</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>214745</xdr:rowOff>
@@ -1092,13 +1155,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>647700</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>86591</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>909205</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -1138,13 +1201,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>28864</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>72158</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>384464</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>144317</xdr:rowOff>
@@ -1192,16 +1255,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>462973</xdr:colOff>
       <xdr:row>5</xdr:row>
+      <xdr:rowOff>19243</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1443182</xdr:colOff>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>28863</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>880341</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>43295</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1209,9 +1272,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7491268" y="1082386"/>
-          <a:ext cx="2899641" cy="14432"/>
+        <a:xfrm flipV="1">
+          <a:off x="10199640" y="1077576"/>
+          <a:ext cx="3712633" cy="9620"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1493,187 +1556,322 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:M29"/>
+  <dimension ref="B1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="66" workbookViewId="0">
+      <selection activeCell="N44" sqref="N44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
-    <col min="10" max="10" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="11" max="11" width="26.85546875" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="F2" s="3" t="s">
+    <row r="1" spans="4:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="4:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="G4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="K4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="4:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="K5" s="4"/>
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="4:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="F4" s="1" t="s">
+      <c r="H6" s="9"/>
+      <c r="K6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="G7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="4:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="G9" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="4:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="4:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="4:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="7"/>
+      <c r="F17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="J17" s="7"/>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="4:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="6"/>
+      <c r="F18" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="L18" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="4:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="4:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="4:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="4:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="L23" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="4:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L24" s="4"/>
+    </row>
+    <row r="25" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="L25" s="8"/>
+    </row>
+    <row r="26" spans="4:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L26" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="F27" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="4:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="4:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F29" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B40" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="J41" s="7"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B45" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="J4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F5" s="5" t="s">
+      <c r="D45" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="J5" s="4"/>
-      <c r="M5" s="4"/>
-    </row>
-    <row r="6" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F6" s="2" t="s">
+      <c r="D46" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B47" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="J6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="F7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="F9" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F10" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="3:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="7"/>
-      <c r="E17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="I17" s="7"/>
-      <c r="K17" s="4"/>
-    </row>
-    <row r="18" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="6"/>
-      <c r="E18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I18" s="1"/>
-      <c r="K18" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E22" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="K23" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K24" s="4"/>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="K25" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K26" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="E27" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="3:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E29" s="2" t="s">
-        <v>10</v>
+      <c r="D48" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>